<commit_message>
añadiendo un profe a la carga automatica del grupo
</commit_message>
<xml_diff>
--- a/grupos.xlsx
+++ b/grupos.xlsx
@@ -20,34 +20,77 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t xml:space="preserve">A</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+  <si>
+    <t xml:space="preserve">B</t>
   </si>
   <si>
     <t xml:space="preserve">ENGLISH</t>
   </si>
   <si>
-    <t xml:space="preserve">alfredo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gonzalez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gaviña</t>
+    <t xml:space="preserve">Rodolfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reyes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martinez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">re@ugto.mx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Franco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25/01/2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">er@ugto.mx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LISC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elizabet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cruz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Garcia</t>
   </si>
   <si>
     <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bautista</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perez</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -68,6 +111,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -112,8 +162,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -134,10 +200,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -146,24 +212,29 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="n">
+      <c r="C1" s="1" t="n">
         <v>3</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>909759</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="n">
+        <v>102358</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="0" t="s">
@@ -172,8 +243,82 @@
       <c r="E3" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="F3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>569878</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>805978</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>205689</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" display="re@ugto.mx"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
desconectando los alumnos de los grupos
</commit_message>
<xml_diff>
--- a/grupos.xlsx
+++ b/grupos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t xml:space="preserve">B</t>
   </si>
@@ -80,6 +80,15 @@
   </si>
   <si>
     <t xml:space="preserve">Perez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arturo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ledezma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">macias</t>
   </si>
 </sst>
 </file>
@@ -200,10 +209,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -314,6 +323,32 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>146824</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>